<commit_message>
KingdomObj -> KingdomItem 이름 변경 / Kindom 관련 api 패킷 생성
</commit_message>
<xml_diff>
--- a/Data/Excel/Enum/Enum.xlsx
+++ b/Data/Excel/Enum/Enum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Enum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C320EBD-77EE-47A1-AA29-D5ABE632075D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E190B55-5B55-419C-A8C3-F8EEB6B27176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="285" windowWidth="12750" windowHeight="11295" activeTab="2" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
+    <workbookView xWindow="705" yWindow="975" windowWidth="13785" windowHeight="11295" activeTab="3" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="1" r:id="rId1"/>
@@ -132,10 +132,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>EKingdomObjType</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>STRUCTURE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -148,10 +144,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>EKingdomObjState</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>CONSTRUCTING</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -168,10 +160,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>EKingdomObjSpecialType</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>FORGE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -252,11 +240,23 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>KINGDOM_OBJ</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>EChannelType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EKingdomItemState</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EKingdomItemSpecialType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EKingdomItemType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>KINGDOM_ITEM</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1197,7 +1197,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A7:B11"/>
+      <selection activeCell="A6" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1246,10 +1246,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1257,10 +1257,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1268,10 +1268,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -1290,10 +1290,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1301,10 +1301,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
         <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1316,10 +1316,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -1327,10 +1327,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -1353,10 +1353,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -1379,10 +1379,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1403,10 +1403,13 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1424,7 +1427,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -1435,10 +1438,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1446,10 +1449,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1457,10 +1460,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
         <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -1468,10 +1471,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -1479,10 +1482,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -1490,10 +1493,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -1501,10 +1504,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C9">
         <v>101</v>
@@ -1512,10 +1515,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10">
         <v>111</v>
@@ -1523,10 +1526,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C11">
         <v>112</v>
@@ -1534,10 +1537,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12">
         <v>113</v>
@@ -1545,10 +1548,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C13">
         <v>200</v>
@@ -1556,10 +1559,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C14">
         <v>200</v>
@@ -1567,10 +1570,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C15">
         <v>201</v>
@@ -1578,10 +1581,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C16">
         <v>300</v>
@@ -1589,10 +1592,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C17">
         <v>1000</v>
@@ -1600,10 +1603,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C18">
         <v>10000</v>
@@ -1611,10 +1614,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C19">
         <v>100000</v>
@@ -1630,7 +1633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E03D05-3359-4F98-AFB8-8B86CD4E3336}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1732,7 +1735,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -1743,7 +1746,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
@@ -1817,8 +1820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39863D74-8F6A-4DBA-9900-ED18DEBD4CDC}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Kingdom 관련 모델 개편 (KingdomDeco, Structure, TIleMap) / ItemModel 추가
</commit_message>
<xml_diff>
--- a/Data/Excel/Enum/Enum.xlsx
+++ b/Data/Excel/Enum/Enum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Enum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E190B55-5B55-419C-A8C3-F8EEB6B27176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB497ED4-5AFD-4AE2-9B13-4C28DFAE6F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="975" windowWidth="13785" windowHeight="11295" activeTab="3" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,23 @@
     <sheet name="Auth" sheetId="3" r:id="rId3"/>
     <sheet name="ErrorCode" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
   <si>
     <t>#</t>
   </si>
@@ -136,10 +147,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>DECORATION</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>TRASH</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -152,10 +159,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>IN_PROGRESS</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>STORED</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -180,10 +183,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>STAR_CANDY</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>FREE_CASH</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -257,6 +256,50 @@
   </si>
   <si>
     <t>KINGDOM_ITEM</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EKingdomTileMapState</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DECO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EKingdomStructureFlagType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUILD</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EPlacedKingdomItemState</t>
+  </si>
+  <si>
+    <t>DELETED</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EItemType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONSUMABLE</t>
+  </si>
+  <si>
+    <t>CRAFTING</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RELIC</t>
+  </si>
+  <si>
+    <t>FUNCTIONAL</t>
+  </si>
+  <si>
+    <t>EXP</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1194,20 +1237,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A4:A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1221,7 +1264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1229,9 +1272,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1244,9 +1287,9 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
@@ -1255,31 +1298,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>57</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -1288,23 +1331,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1314,23 +1357,23 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -1340,9 +1383,9 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -1351,12 +1394,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1366,9 +1409,9 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -1377,12 +1420,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1391,6 +1434,116 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -1402,16 +1555,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750CB274-E046-4C1F-A936-2BBE6C493CFE}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1425,9 +1578,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -1436,188 +1589,188 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C14">
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C15">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C16">
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17">
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C18">
         <v>10000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C19">
         <v>100000</v>
@@ -1637,12 +1790,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1656,7 +1809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1667,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1678,7 +1831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1689,7 +1842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1700,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1711,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1722,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1733,9 +1886,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -1744,9 +1897,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
@@ -1755,7 +1908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1766,7 +1919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1777,7 +1930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1788,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1799,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1820,17 +1973,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39863D74-8F6A-4DBA-9900-ED18DEBD4CDC}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1844,7 +1997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1855,7 +2008,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1866,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1877,7 +2030,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1888,7 +2041,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1899,7 +2052,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1910,7 +2063,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1921,7 +2074,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1932,7 +2085,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1943,7 +2096,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Schedule 관련 Proto 생성 / ProtoGenerater 복합 pk, list 읽기 작업
</commit_message>
<xml_diff>
--- a/Data/Excel/Enum/Enum.xlsx
+++ b/Data/Excel/Enum/Enum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Enum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ECA9FB-22F2-4AFE-BD23-009B073D159F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57812F2-5725-4018-98FD-591EFE90C683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="91">
   <si>
     <t>#</t>
   </si>
@@ -380,6 +380,18 @@
   </si>
   <si>
     <t>REAR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EScheduleType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GACHA</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATTENDANCE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1317,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1843,6 +1855,39 @@
       </c>
       <c r="C45">
         <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CenterDb 추가 / CookieSoulStone 추가 / Log 성 테이블 추가
</commit_message>
<xml_diff>
--- a/Data/Excel/Enum/Enum.xlsx
+++ b/Data/Excel/Enum/Enum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Enum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57812F2-5725-4018-98FD-591EFE90C683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CACE071-52CF-41CF-9802-139F9891B43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="93">
   <si>
     <t>#</t>
   </si>
@@ -392,6 +392,14 @@
   </si>
   <si>
     <t>ATTENDANCE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ECookieSoulStoneType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOUL_STONE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1329,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1529,40 +1537,44 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
+        <v>91</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>60</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>58</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -1571,20 +1583,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>58</v>
-      </c>
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>62</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
@@ -1593,147 +1605,147 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>62</v>
       </c>
       <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
         <v>64</v>
       </c>
-      <c r="C25">
+      <c r="C27">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="C28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1741,10 +1753,10 @@
         <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1752,10 +1764,10 @@
         <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1763,10 +1775,10 @@
         <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1774,10 +1786,10 @@
         <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1785,10 +1797,10 @@
         <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C39">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1796,10 +1808,10 @@
         <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C40">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1807,32 +1819,32 @@
         <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C41">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1840,10 +1852,10 @@
         <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1851,32 +1863,32 @@
         <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C47">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1884,9 +1896,31 @@
         <v>88</v>
       </c>
       <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" t="s">
         <v>90</v>
       </c>
-      <c r="C48">
+      <c r="C50">
         <v>20</v>
       </c>
     </row>
@@ -1898,10 +1932,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750CB274-E046-4C1F-A936-2BBE6C493CFE}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2104,10 +2138,10 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="C18">
-        <v>10000</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2115,9 +2149,20 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
         <v>55</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>100000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cookie Enhance Lv, Star api 작성
</commit_message>
<xml_diff>
--- a/Data/Excel/Enum/Enum.xlsx
+++ b/Data/Excel/Enum/Enum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Enum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB05564B-648E-4B21-905A-66924751B437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1CD791-78E9-44B1-86D1-FB9FA388C4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="3255" windowWidth="22980" windowHeight="11295" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
+    <workbookView xWindow="1680" yWindow="3435" windowWidth="22980" windowHeight="11295" activeTab="1" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="101">
   <si>
     <t>#</t>
   </si>
@@ -428,6 +428,10 @@
   </si>
   <si>
     <t>SPECIAL</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>POINT_COOKIE_LV</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1367,7 +1371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
@@ -2037,10 +2041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750CB274-E046-4C1F-A936-2BBE6C493CFE}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2155,10 +2159,10 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="C10">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2166,10 +2170,10 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2177,10 +2181,10 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2188,10 +2192,10 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13">
-        <v>200</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2199,7 +2203,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14">
         <v>200</v>
@@ -2210,10 +2214,10 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2221,10 +2225,10 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16">
-        <v>300</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2232,10 +2236,10 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17">
-        <v>1000</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2243,10 +2247,10 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="C18">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2254,10 +2258,10 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="C19">
-        <v>10000</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2265,9 +2269,20 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
         <v>55</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>100000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WorldStage 관련 Prt, Model 설계
</commit_message>
<xml_diff>
--- a/Data/Excel/Enum/Enum.xlsx
+++ b/Data/Excel/Enum/Enum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Enum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1CD791-78E9-44B1-86D1-FB9FA388C4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1679FE5-5E5F-4AE2-851A-395D2BD93770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="3435" windowWidth="22980" windowHeight="11295" activeTab="1" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="108">
   <si>
     <t>#</t>
   </si>
@@ -432,6 +432,34 @@
   </si>
   <si>
     <t>POINT_COOKIE_LV</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EWorldType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NORMAL</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DARK</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MASTER</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EWorldStageType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>STAGE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>VILLAGE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1369,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D64" sqref="D60:E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2033,6 +2061,72 @@
         <v>2</v>
       </c>
     </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B58" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2043,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750CB274-E046-4C1F-A936-2BBE6C493CFE}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>

</xml_diff>